<commit_message>
updated w volt regulator missing on MCU PCB
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Hydration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B12E63A-2830-48BF-AC3A-BB6311307E76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0470DB64-D9BE-4225-829D-C0307D794463}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{C3AD9D2E-3E69-485C-A23B-91E4490D16E1}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="377">
   <si>
     <t>Item#</t>
   </si>
@@ -1224,6 +1224,9 @@
   </si>
   <si>
     <t>AD8606 - Op Amp</t>
+  </si>
+  <si>
+    <t>AP2112K-3.3 Voltage Regulator</t>
   </si>
 </sst>
 </file>
@@ -1931,7 +1934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="211">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2484,6 +2487,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4035,10 +4044,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D154C8AB-27F7-4A13-8063-275E3E6867F6}">
-  <dimension ref="A1:AD92"/>
+  <dimension ref="A1:AD93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5112,77 +5121,74 @@
       <c r="AB27" s="102"/>
       <c r="AC27" s="109"/>
     </row>
-    <row r="28" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="194"/>
-      <c r="B28" s="140" t="s">
-        <v>211</v>
-      </c>
-      <c r="C28" s="138">
+    <row r="28" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="188"/>
+      <c r="B28" s="81" t="s">
+        <v>376</v>
+      </c>
+      <c r="C28" s="212">
         <v>1</v>
       </c>
-      <c r="D28" s="138">
-        <v>4</v>
-      </c>
-      <c r="E28" s="142" t="s">
-        <v>212</v>
+      <c r="D28" s="212">
+        <v>0</v>
+      </c>
+      <c r="E28" s="82" t="s">
+        <v>268</v>
       </c>
       <c r="F28" s="134"/>
-      <c r="L28" s="210"/>
-      <c r="M28" s="116" t="s">
-        <v>364</v>
-      </c>
-      <c r="N28" s="117">
-        <v>1</v>
-      </c>
-      <c r="O28" s="117">
-        <v>4</v>
-      </c>
-      <c r="P28" s="118" t="s">
-        <v>219</v>
-      </c>
+      <c r="L28" s="211"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="54"/>
       <c r="Q28" s="45"/>
-      <c r="V28" s="108" t="s">
-        <v>202</v>
-      </c>
-      <c r="W28" s="102" t="s">
-        <v>131</v>
-      </c>
-      <c r="X28" s="102" t="s">
-        <v>131</v>
-      </c>
+      <c r="V28" s="108"/>
+      <c r="W28" s="102"/>
+      <c r="X28" s="102"/>
       <c r="Y28" s="102"/>
       <c r="Z28" s="102"/>
       <c r="AA28" s="102"/>
       <c r="AB28" s="102"/>
       <c r="AC28" s="109"/>
     </row>
-    <row r="29" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="188" t="s">
-        <v>213</v>
-      </c>
-      <c r="B29" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="C29" s="36">
+    <row r="29" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="194"/>
+      <c r="B29" s="140" t="s">
+        <v>211</v>
+      </c>
+      <c r="C29" s="138">
         <v>1</v>
       </c>
-      <c r="D29" s="36">
+      <c r="D29" s="138">
         <v>4</v>
       </c>
-      <c r="E29" s="48" t="s">
-        <v>215</v>
+      <c r="E29" s="142" t="s">
+        <v>212</v>
       </c>
       <c r="F29" s="134"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="51"/>
-      <c r="P29" s="55"/>
+      <c r="L29" s="210"/>
+      <c r="M29" s="116" t="s">
+        <v>364</v>
+      </c>
+      <c r="N29" s="117">
+        <v>1</v>
+      </c>
+      <c r="O29" s="117">
+        <v>4</v>
+      </c>
+      <c r="P29" s="118" t="s">
+        <v>219</v>
+      </c>
       <c r="Q29" s="45"/>
-      <c r="V29" s="108"/>
-      <c r="W29" s="102"/>
-      <c r="X29" s="102"/>
+      <c r="V29" s="108" t="s">
+        <v>202</v>
+      </c>
+      <c r="W29" s="102" t="s">
+        <v>131</v>
+      </c>
+      <c r="X29" s="102" t="s">
+        <v>131</v>
+      </c>
       <c r="Y29" s="102"/>
       <c r="Z29" s="102"/>
       <c r="AA29" s="102"/>
@@ -5190,30 +5196,30 @@
       <c r="AC29" s="109"/>
     </row>
     <row r="30" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="188"/>
+      <c r="A30" s="188" t="s">
+        <v>213</v>
+      </c>
       <c r="B30" s="27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C30" s="36">
         <v>1</v>
       </c>
-      <c r="D30" s="34" t="s">
-        <v>217</v>
+      <c r="D30" s="36">
+        <v>4</v>
       </c>
       <c r="E30" s="48" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F30" s="134"/>
       <c r="K30" s="33"/>
       <c r="L30" s="35"/>
       <c r="M30" s="27"/>
       <c r="N30" s="51"/>
-      <c r="O30" s="50"/>
+      <c r="O30" s="51"/>
       <c r="P30" s="55"/>
       <c r="Q30" s="45"/>
-      <c r="V30" s="108" t="s">
-        <v>213</v>
-      </c>
+      <c r="V30" s="108"/>
       <c r="W30" s="102"/>
       <c r="X30" s="102"/>
       <c r="Y30" s="102"/>
@@ -5223,131 +5229,130 @@
       <c r="AC30" s="109"/>
     </row>
     <row r="31" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="189"/>
-      <c r="B31" s="43" t="s">
-        <v>364</v>
-      </c>
-      <c r="C31" s="44">
+      <c r="A31" s="188"/>
+      <c r="B31" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="C31" s="36">
         <v>1</v>
       </c>
-      <c r="D31" s="44">
-        <v>4</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="F31" s="46"/>
+      <c r="D31" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="E31" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="F31" s="134"/>
       <c r="K31" s="33"/>
       <c r="L31" s="35"/>
-      <c r="M31" s="40"/>
+      <c r="M31" s="27"/>
       <c r="N31" s="51"/>
-      <c r="O31" s="51"/>
+      <c r="O31" s="50"/>
       <c r="P31" s="55"/>
       <c r="Q31" s="45"/>
-      <c r="U31" s="96"/>
       <c r="V31" s="108" t="s">
-        <v>220</v>
-      </c>
-      <c r="W31" s="102" t="s">
-        <v>221</v>
-      </c>
-      <c r="X31" s="102" t="s">
-        <v>222</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="W31" s="102"/>
+      <c r="X31" s="102"/>
       <c r="Y31" s="102"/>
       <c r="Z31" s="102"/>
       <c r="AA31" s="102"/>
       <c r="AB31" s="102"/>
       <c r="AC31" s="109"/>
-      <c r="AD31" s="96"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="42"/>
+    </row>
+    <row r="32" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="189"/>
+      <c r="B32" s="43" t="s">
+        <v>364</v>
+      </c>
+      <c r="C32" s="44">
+        <v>1</v>
+      </c>
+      <c r="D32" s="44">
+        <v>4</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="F32" s="46"/>
       <c r="K32" s="33"/>
-      <c r="L32" s="37"/>
+      <c r="L32" s="35"/>
       <c r="M32" s="40"/>
       <c r="N32" s="51"/>
       <c r="O32" s="51"/>
       <c r="P32" s="55"/>
-      <c r="Q32" s="41"/>
+      <c r="Q32" s="45"/>
       <c r="U32" s="96"/>
-      <c r="V32" s="125" t="s">
+      <c r="V32" s="108" t="s">
+        <v>220</v>
+      </c>
+      <c r="W32" s="102" t="s">
+        <v>221</v>
+      </c>
+      <c r="X32" s="102" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y32" s="102"/>
+      <c r="Z32" s="102"/>
+      <c r="AA32" s="102"/>
+      <c r="AB32" s="102"/>
+      <c r="AC32" s="109"/>
+      <c r="AD32" s="96"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A33" s="37"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="42"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="51"/>
+      <c r="O33" s="51"/>
+      <c r="P33" s="55"/>
+      <c r="Q33" s="41"/>
+      <c r="U33" s="96"/>
+      <c r="V33" s="125" t="s">
         <v>278</v>
       </c>
-      <c r="W32" s="126" t="s">
+      <c r="W33" s="126" t="s">
         <v>335</v>
       </c>
-      <c r="X32" s="127" t="s">
+      <c r="X33" s="127" t="s">
         <v>336</v>
       </c>
-      <c r="Y32" s="126"/>
-      <c r="Z32" s="126"/>
-      <c r="AA32" s="126"/>
-      <c r="AB32" s="126"/>
-      <c r="AC32" s="128"/>
-      <c r="AD32" s="96"/>
-    </row>
-    <row r="33" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="176" t="s">
+      <c r="Y33" s="126"/>
+      <c r="Z33" s="126"/>
+      <c r="AA33" s="126"/>
+      <c r="AB33" s="126"/>
+      <c r="AC33" s="128"/>
+      <c r="AD33" s="96"/>
+    </row>
+    <row r="34" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="176" t="s">
         <v>295</v>
       </c>
-      <c r="C33" s="177"/>
-      <c r="D33" s="177"/>
-      <c r="E33" s="177"/>
-      <c r="F33" s="177"/>
-      <c r="G33" s="177"/>
-      <c r="H33" s="177"/>
-      <c r="I33" s="178"/>
-      <c r="J33" s="146"/>
-      <c r="L33" s="203" t="s">
+      <c r="C34" s="177"/>
+      <c r="D34" s="177"/>
+      <c r="E34" s="177"/>
+      <c r="F34" s="177"/>
+      <c r="G34" s="177"/>
+      <c r="H34" s="177"/>
+      <c r="I34" s="178"/>
+      <c r="J34" s="146"/>
+      <c r="L34" s="203" t="s">
         <v>338</v>
       </c>
-      <c r="M33" s="204"/>
-      <c r="N33" s="204"/>
-      <c r="O33" s="204"/>
-      <c r="P33" s="204"/>
-      <c r="Q33" s="204"/>
-      <c r="R33" s="204"/>
-      <c r="S33" s="205"/>
-      <c r="U33" s="96"/>
-      <c r="V33" s="96"/>
-      <c r="W33" s="96"/>
-      <c r="X33" s="96"/>
-      <c r="Y33" s="96"/>
-      <c r="Z33" s="96"/>
-      <c r="AA33" s="96"/>
-      <c r="AB33" s="96"/>
-      <c r="AC33" s="152"/>
-      <c r="AD33" s="27"/>
-    </row>
-    <row r="34" spans="2:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="33"/>
-      <c r="L34" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="M34" s="68"/>
-      <c r="N34" s="68"/>
-      <c r="O34" s="68"/>
-      <c r="P34" s="68"/>
-      <c r="Q34" s="68"/>
-      <c r="R34" s="68"/>
-      <c r="S34" s="69"/>
-      <c r="T34" s="61"/>
+      <c r="M34" s="204"/>
+      <c r="N34" s="204"/>
+      <c r="O34" s="204"/>
+      <c r="P34" s="204"/>
+      <c r="Q34" s="204"/>
+      <c r="R34" s="204"/>
+      <c r="S34" s="205"/>
       <c r="U34" s="96"/>
       <c r="V34" s="96"/>
       <c r="W34" s="96"/>
@@ -5356,40 +5361,32 @@
       <c r="Z34" s="96"/>
       <c r="AA34" s="96"/>
       <c r="AB34" s="96"/>
-      <c r="AC34" s="96"/>
-      <c r="AD34" s="151"/>
-    </row>
-    <row r="35" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC34" s="152"/>
+      <c r="AD34" s="27"/>
+    </row>
+    <row r="35" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="D35" s="33" t="s">
-        <v>222</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
       <c r="E35" s="33"/>
       <c r="F35" s="33"/>
       <c r="G35" s="33"/>
       <c r="H35" s="33"/>
       <c r="I35" s="30"/>
       <c r="J35" s="33"/>
-      <c r="L35" s="108" t="s">
-        <v>220</v>
-      </c>
-      <c r="M35" s="102" t="s">
-        <v>221</v>
-      </c>
-      <c r="N35" s="102" t="s">
-        <v>222</v>
-      </c>
-      <c r="O35" s="102"/>
-      <c r="P35" s="102"/>
-      <c r="Q35" s="102"/>
-      <c r="R35" s="102"/>
-      <c r="S35" s="109"/>
-      <c r="T35" s="107"/>
+      <c r="L35" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="M35" s="68"/>
+      <c r="N35" s="68"/>
+      <c r="O35" s="68"/>
+      <c r="P35" s="68"/>
+      <c r="Q35" s="68"/>
+      <c r="R35" s="68"/>
+      <c r="S35" s="69"/>
+      <c r="T35" s="61"/>
       <c r="U35" s="96"/>
       <c r="V35" s="96"/>
       <c r="W35" s="96"/>
@@ -5399,32 +5396,32 @@
       <c r="AA35" s="96"/>
       <c r="AB35" s="96"/>
       <c r="AC35" s="96"/>
-      <c r="AD35" s="107"/>
-    </row>
-    <row r="36" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="80" t="s">
-        <v>223</v>
-      </c>
-      <c r="C36" s="81" t="s">
-        <v>224</v>
-      </c>
-      <c r="D36" s="81" t="s">
-        <v>225</v>
-      </c>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="82"/>
-      <c r="J36" s="27"/>
+      <c r="AD35" s="151"/>
+    </row>
+    <row r="36" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="33"/>
       <c r="L36" s="108" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M36" s="102" t="s">
-        <v>231</v>
-      </c>
-      <c r="N36" s="110" t="s">
-        <v>229</v>
+        <v>221</v>
+      </c>
+      <c r="N36" s="102" t="s">
+        <v>222</v>
       </c>
       <c r="O36" s="102"/>
       <c r="P36" s="102"/>
@@ -5433,12 +5430,19 @@
       <c r="S36" s="109"/>
       <c r="T36" s="107"/>
       <c r="U36" s="96"/>
+      <c r="V36" s="96"/>
+      <c r="W36" s="96"/>
+      <c r="X36" s="96"/>
+      <c r="Y36" s="96"/>
+      <c r="Z36" s="96"/>
+      <c r="AA36" s="96"/>
+      <c r="AB36" s="96"/>
       <c r="AC36" s="96"/>
       <c r="AD36" s="107"/>
     </row>
-    <row r="37" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="80" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C37" s="81" t="s">
         <v>224</v>
@@ -5453,7 +5457,7 @@
       <c r="I37" s="82"/>
       <c r="J37" s="27"/>
       <c r="L37" s="108" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="M37" s="102" t="s">
         <v>231</v>
@@ -5468,30 +5472,30 @@
       <c r="S37" s="109"/>
       <c r="T37" s="107"/>
       <c r="U37" s="96"/>
+      <c r="AC37" s="96"/>
       <c r="AD37" s="107"/>
     </row>
-    <row r="38" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="90" t="s">
-        <v>227</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="48"/>
+    <row r="38" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="C38" s="81" t="s">
+        <v>224</v>
+      </c>
+      <c r="D38" s="81" t="s">
+        <v>225</v>
+      </c>
+      <c r="E38" s="81"/>
+      <c r="F38" s="81"/>
+      <c r="G38" s="81"/>
+      <c r="H38" s="81"/>
+      <c r="I38" s="82"/>
       <c r="J38" s="27"/>
-      <c r="K38" s="96"/>
       <c r="L38" s="108" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M38" s="102" t="s">
-        <v>297</v>
+        <v>231</v>
       </c>
       <c r="N38" s="110" t="s">
         <v>229</v>
@@ -5505,9 +5509,9 @@
       <c r="U38" s="96"/>
       <c r="AD38" s="107"/>
     </row>
-    <row r="39" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="90" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C39" s="27" t="s">
         <v>228</v>
@@ -5523,10 +5527,10 @@
       <c r="J39" s="27"/>
       <c r="K39" s="96"/>
       <c r="L39" s="108" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="M39" s="102" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="N39" s="110" t="s">
         <v>229</v>
@@ -5540,12 +5544,12 @@
       <c r="U39" s="96"/>
       <c r="AD39" s="107"/>
     </row>
-    <row r="40" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="90" t="s">
-        <v>179</v>
+        <v>230</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D40" s="27" t="s">
         <v>229</v>
@@ -5558,7 +5562,7 @@
       <c r="J40" s="27"/>
       <c r="K40" s="96"/>
       <c r="L40" s="108" t="s">
-        <v>179</v>
+        <v>230</v>
       </c>
       <c r="M40" s="102" t="s">
         <v>298</v>
@@ -5575,12 +5579,12 @@
       <c r="U40" s="96"/>
       <c r="AD40" s="107"/>
     </row>
-    <row r="41" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="90" t="s">
-        <v>232</v>
+        <v>179</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D41" s="27" t="s">
         <v>229</v>
@@ -5593,7 +5597,7 @@
       <c r="J41" s="27"/>
       <c r="K41" s="96"/>
       <c r="L41" s="108" t="s">
-        <v>232</v>
+        <v>179</v>
       </c>
       <c r="M41" s="102" t="s">
         <v>298</v>
@@ -5606,16 +5610,16 @@
       <c r="Q41" s="102"/>
       <c r="R41" s="102"/>
       <c r="S41" s="109"/>
-      <c r="T41" s="61"/>
+      <c r="T41" s="107"/>
       <c r="U41" s="96"/>
       <c r="AD41" s="107"/>
     </row>
-    <row r="42" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="90" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="D42" s="27" t="s">
         <v>229</v>
@@ -5628,7 +5632,7 @@
       <c r="J42" s="27"/>
       <c r="K42" s="96"/>
       <c r="L42" s="108" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M42" s="102" t="s">
         <v>298</v>
@@ -5645,9 +5649,9 @@
       <c r="U42" s="96"/>
       <c r="AD42" s="107"/>
     </row>
-    <row r="43" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="90" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C43" s="27" t="s">
         <v>228</v>
@@ -5663,10 +5667,10 @@
       <c r="J43" s="27"/>
       <c r="K43" s="96"/>
       <c r="L43" s="108" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M43" s="102" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="N43" s="110" t="s">
         <v>229</v>
@@ -5680,12 +5684,12 @@
       <c r="U43" s="96"/>
       <c r="AD43" s="107"/>
     </row>
-    <row r="44" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="90" t="s">
-        <v>174</v>
+        <v>235</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D44" s="27" t="s">
         <v>229</v>
@@ -5698,10 +5702,10 @@
       <c r="J44" s="27"/>
       <c r="K44" s="96"/>
       <c r="L44" s="108" t="s">
-        <v>174</v>
+        <v>235</v>
       </c>
       <c r="M44" s="102" t="s">
-        <v>228</v>
+        <v>297</v>
       </c>
       <c r="N44" s="110" t="s">
         <v>229</v>
@@ -5715,12 +5719,12 @@
       <c r="U44" s="96"/>
       <c r="AD44" s="107"/>
     </row>
-    <row r="45" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="90" t="s">
-        <v>237</v>
+        <v>174</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D45" s="27" t="s">
         <v>229</v>
@@ -5733,13 +5737,13 @@
       <c r="J45" s="27"/>
       <c r="K45" s="96"/>
       <c r="L45" s="108" t="s">
-        <v>237</v>
+        <v>174</v>
       </c>
       <c r="M45" s="102" t="s">
-        <v>299</v>
+        <v>228</v>
       </c>
       <c r="N45" s="110" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="O45" s="102"/>
       <c r="P45" s="102"/>
@@ -5750,9 +5754,9 @@
       <c r="U45" s="96"/>
       <c r="AD45" s="107"/>
     </row>
-    <row r="46" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="90" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C46" s="27" t="s">
         <v>238</v>
@@ -5768,13 +5772,13 @@
       <c r="J46" s="27"/>
       <c r="K46" s="96"/>
       <c r="L46" s="108" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="M46" s="102" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N46" s="110" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="O46" s="102"/>
       <c r="P46" s="102"/>
@@ -5785,12 +5789,12 @@
       <c r="U46" s="96"/>
       <c r="AD46" s="107"/>
     </row>
-    <row r="47" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="90" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D47" s="27" t="s">
         <v>229</v>
@@ -5803,10 +5807,10 @@
       <c r="J47" s="27"/>
       <c r="K47" s="96"/>
       <c r="L47" s="108" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M47" s="102" t="s">
-        <v>238</v>
+        <v>300</v>
       </c>
       <c r="N47" s="110" t="s">
         <v>229</v>
@@ -5820,9 +5824,9 @@
       <c r="U47" s="96"/>
       <c r="AD47" s="107"/>
     </row>
-    <row r="48" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="90" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C48" s="27" t="s">
         <v>241</v>
@@ -5838,7 +5842,7 @@
       <c r="J48" s="27"/>
       <c r="K48" s="96"/>
       <c r="L48" s="108" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M48" s="102" t="s">
         <v>238</v>
@@ -5857,10 +5861,10 @@
     </row>
     <row r="49" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="90" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="D49" s="27" t="s">
         <v>229</v>
@@ -5873,10 +5877,10 @@
       <c r="J49" s="27"/>
       <c r="K49" s="96"/>
       <c r="L49" s="108" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M49" s="102" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="N49" s="110" t="s">
         <v>229</v>
@@ -5892,7 +5896,7 @@
     </row>
     <row r="50" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="90" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C50" s="27" t="s">
         <v>233</v>
@@ -5908,10 +5912,10 @@
       <c r="J50" s="27"/>
       <c r="K50" s="96"/>
       <c r="L50" s="108" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M50" s="102" t="s">
-        <v>301</v>
+        <v>228</v>
       </c>
       <c r="N50" s="110" t="s">
         <v>229</v>
@@ -5927,10 +5931,10 @@
     </row>
     <row r="51" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="90" t="s">
-        <v>170</v>
+        <v>244</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="D51" s="27" t="s">
         <v>229</v>
@@ -5943,10 +5947,10 @@
       <c r="J51" s="27"/>
       <c r="K51" s="96"/>
       <c r="L51" s="108" t="s">
-        <v>170</v>
+        <v>244</v>
       </c>
       <c r="M51" s="102" t="s">
-        <v>238</v>
+        <v>301</v>
       </c>
       <c r="N51" s="110" t="s">
         <v>229</v>
@@ -5958,12 +5962,18 @@
       <c r="S51" s="109"/>
       <c r="T51" s="61"/>
       <c r="U51" s="96"/>
-      <c r="AD51" s="96"/>
+      <c r="AD51" s="107"/>
     </row>
     <row r="52" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="90"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
+      <c r="B52" s="90" t="s">
+        <v>170</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>229</v>
+      </c>
       <c r="E52" s="27"/>
       <c r="F52" s="27"/>
       <c r="G52" s="27"/>
@@ -5971,9 +5981,15 @@
       <c r="I52" s="48"/>
       <c r="J52" s="27"/>
       <c r="K52" s="96"/>
-      <c r="L52" s="108"/>
-      <c r="M52" s="102"/>
-      <c r="N52" s="102"/>
+      <c r="L52" s="108" t="s">
+        <v>170</v>
+      </c>
+      <c r="M52" s="102" t="s">
+        <v>238</v>
+      </c>
+      <c r="N52" s="110" t="s">
+        <v>229</v>
+      </c>
       <c r="O52" s="102"/>
       <c r="P52" s="102"/>
       <c r="Q52" s="102"/>
@@ -5984,9 +6000,7 @@
       <c r="AD52" s="96"/>
     </row>
     <row r="53" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="90" t="s">
-        <v>36</v>
-      </c>
+      <c r="B53" s="90"/>
       <c r="C53" s="27"/>
       <c r="D53" s="27"/>
       <c r="E53" s="27"/>
@@ -5996,9 +6010,7 @@
       <c r="I53" s="48"/>
       <c r="J53" s="27"/>
       <c r="K53" s="96"/>
-      <c r="L53" s="111" t="s">
-        <v>36</v>
-      </c>
+      <c r="L53" s="108"/>
       <c r="M53" s="102"/>
       <c r="N53" s="102"/>
       <c r="O53" s="102"/>
@@ -6012,14 +6024,10 @@
     </row>
     <row r="54" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="90" t="s">
-        <v>220</v>
-      </c>
-      <c r="C54" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="D54" s="27" t="s">
-        <v>222</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
       <c r="E54" s="27"/>
       <c r="F54" s="27"/>
       <c r="G54" s="27"/>
@@ -6027,31 +6035,29 @@
       <c r="I54" s="48"/>
       <c r="J54" s="27"/>
       <c r="K54" s="96"/>
-      <c r="L54" s="108" t="s">
-        <v>220</v>
-      </c>
-      <c r="M54" s="102" t="s">
-        <v>221</v>
-      </c>
-      <c r="N54" s="102" t="s">
-        <v>302</v>
-      </c>
+      <c r="L54" s="111" t="s">
+        <v>36</v>
+      </c>
+      <c r="M54" s="102"/>
+      <c r="N54" s="102"/>
       <c r="O54" s="102"/>
       <c r="P54" s="102"/>
       <c r="Q54" s="102"/>
       <c r="R54" s="102"/>
       <c r="S54" s="109"/>
       <c r="T54" s="61"/>
+      <c r="U54" s="96"/>
+      <c r="AD54" s="96"/>
     </row>
     <row r="55" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="90" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="E55" s="27"/>
       <c r="F55" s="27"/>
@@ -6061,13 +6067,13 @@
       <c r="J55" s="27"/>
       <c r="K55" s="96"/>
       <c r="L55" s="108" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="M55" s="102" t="s">
-        <v>249</v>
-      </c>
-      <c r="N55" s="110" t="s">
-        <v>247</v>
+        <v>221</v>
+      </c>
+      <c r="N55" s="102" t="s">
+        <v>302</v>
       </c>
       <c r="O55" s="102"/>
       <c r="P55" s="102"/>
@@ -6078,10 +6084,10 @@
     </row>
     <row r="56" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="90" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D56" s="27" t="s">
         <v>247</v>
@@ -6094,10 +6100,10 @@
       <c r="J56" s="27"/>
       <c r="K56" s="96"/>
       <c r="L56" s="108" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="M56" s="102" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="N56" s="110" t="s">
         <v>247</v>
@@ -6111,7 +6117,7 @@
     </row>
     <row r="57" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="90" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C57" s="27" t="s">
         <v>249</v>
@@ -6127,7 +6133,7 @@
       <c r="J57" s="27"/>
       <c r="K57" s="96"/>
       <c r="L57" s="108" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M57" s="102" t="s">
         <v>255</v>
@@ -6144,7 +6150,7 @@
     </row>
     <row r="58" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="90" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C58" s="27" t="s">
         <v>249</v>
@@ -6160,7 +6166,7 @@
       <c r="J58" s="27"/>
       <c r="K58" s="96"/>
       <c r="L58" s="108" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M58" s="102" t="s">
         <v>255</v>
@@ -6177,7 +6183,7 @@
     </row>
     <row r="59" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="90" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C59" s="27" t="s">
         <v>249</v>
@@ -6193,7 +6199,7 @@
       <c r="J59" s="27"/>
       <c r="K59" s="96"/>
       <c r="L59" s="108" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M59" s="102" t="s">
         <v>255</v>
@@ -6210,10 +6216,10 @@
     </row>
     <row r="60" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="90" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D60" s="27" t="s">
         <v>247</v>
@@ -6226,7 +6232,7 @@
       <c r="J60" s="27"/>
       <c r="K60" s="96"/>
       <c r="L60" s="108" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M60" s="102" t="s">
         <v>255</v>
@@ -6239,14 +6245,14 @@
       <c r="Q60" s="102"/>
       <c r="R60" s="102"/>
       <c r="S60" s="109"/>
-      <c r="T60" s="107"/>
+      <c r="T60" s="61"/>
     </row>
     <row r="61" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="90" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D61" s="27" t="s">
         <v>247</v>
@@ -6259,7 +6265,7 @@
       <c r="J61" s="27"/>
       <c r="K61" s="96"/>
       <c r="L61" s="108" t="s">
-        <v>187</v>
+        <v>254</v>
       </c>
       <c r="M61" s="102" t="s">
         <v>255</v>
@@ -6276,10 +6282,10 @@
     </row>
     <row r="62" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="90" t="s">
-        <v>187</v>
+        <v>254</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D62" s="27" t="s">
         <v>247</v>
@@ -6292,10 +6298,10 @@
       <c r="J62" s="27"/>
       <c r="K62" s="96"/>
       <c r="L62" s="108" t="s">
-        <v>303</v>
+        <v>187</v>
       </c>
       <c r="M62" s="102" t="s">
-        <v>304</v>
+        <v>255</v>
       </c>
       <c r="N62" s="110" t="s">
         <v>247</v>
@@ -6308,21 +6314,27 @@
       <c r="T62" s="107"/>
     </row>
     <row r="63" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="32"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
-      <c r="H63" s="33"/>
-      <c r="I63" s="30"/>
-      <c r="J63" s="33"/>
+      <c r="B63" s="90" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
+      <c r="I63" s="48"/>
+      <c r="J63" s="27"/>
       <c r="K63" s="96"/>
       <c r="L63" s="108" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M63" s="102" t="s">
-        <v>255</v>
+        <v>304</v>
       </c>
       <c r="N63" s="110" t="s">
         <v>247</v>
@@ -6335,9 +6347,7 @@
       <c r="T63" s="107"/>
     </row>
     <row r="64" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="32" t="s">
-        <v>256</v>
-      </c>
+      <c r="B64" s="32"/>
       <c r="C64" s="33"/>
       <c r="D64" s="33"/>
       <c r="E64" s="33"/>
@@ -6348,7 +6358,7 @@
       <c r="J64" s="33"/>
       <c r="K64" s="96"/>
       <c r="L64" s="108" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M64" s="102" t="s">
         <v>255</v>
@@ -6365,14 +6375,10 @@
     </row>
     <row r="65" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="C65" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="D65" s="33" t="s">
-        <v>222</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
       <c r="E65" s="33"/>
       <c r="F65" s="33"/>
       <c r="G65" s="33"/>
@@ -6381,7 +6387,7 @@
       <c r="J65" s="33"/>
       <c r="K65" s="96"/>
       <c r="L65" s="108" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M65" s="102" t="s">
         <v>255</v>
@@ -6398,13 +6404,13 @@
     </row>
     <row r="66" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="32" t="s">
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="C66" s="33" t="s">
-        <v>257</v>
+        <v>221</v>
       </c>
       <c r="D66" s="33" t="s">
-        <v>258</v>
+        <v>222</v>
       </c>
       <c r="E66" s="33"/>
       <c r="F66" s="33"/>
@@ -6414,7 +6420,7 @@
       <c r="J66" s="33"/>
       <c r="K66" s="96"/>
       <c r="L66" s="108" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M66" s="102" t="s">
         <v>255</v>
@@ -6431,13 +6437,13 @@
     </row>
     <row r="67" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="32" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C67" s="33" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D67" s="33" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E67" s="33"/>
       <c r="F67" s="33"/>
@@ -6447,10 +6453,10 @@
       <c r="J67" s="33"/>
       <c r="K67" s="96"/>
       <c r="L67" s="108" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M67" s="102" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="N67" s="110" t="s">
         <v>247</v>
@@ -6464,13 +6470,13 @@
     </row>
     <row r="68" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="32" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C68" s="33" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D68" s="33" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E68" s="33"/>
       <c r="F68" s="33"/>
@@ -6480,10 +6486,10 @@
       <c r="J68" s="33"/>
       <c r="K68" s="96"/>
       <c r="L68" s="108" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M68" s="102" t="s">
-        <v>311</v>
+        <v>249</v>
       </c>
       <c r="N68" s="110" t="s">
         <v>247</v>
@@ -6497,13 +6503,13 @@
     </row>
     <row r="69" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="32" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D69" s="33" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E69" s="33"/>
       <c r="F69" s="33"/>
@@ -6513,10 +6519,10 @@
       <c r="J69" s="33"/>
       <c r="K69" s="96"/>
       <c r="L69" s="108" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="M69" s="102" t="s">
-        <v>249</v>
+        <v>311</v>
       </c>
       <c r="N69" s="110" t="s">
         <v>247</v>
@@ -6530,13 +6536,13 @@
     </row>
     <row r="70" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="32" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C70" s="33" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D70" s="33" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E70" s="33"/>
       <c r="F70" s="33"/>
@@ -6546,7 +6552,7 @@
       <c r="J70" s="33"/>
       <c r="K70" s="96"/>
       <c r="L70" s="108" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M70" s="102" t="s">
         <v>249</v>
@@ -6562,9 +6568,15 @@
       <c r="T70" s="107"/>
     </row>
     <row r="71" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="32"/>
-      <c r="C71" s="33"/>
-      <c r="D71" s="33"/>
+      <c r="B71" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="C71" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="D71" s="33" t="s">
+        <v>266</v>
+      </c>
       <c r="E71" s="33"/>
       <c r="F71" s="33"/>
       <c r="G71" s="33"/>
@@ -6573,10 +6585,10 @@
       <c r="J71" s="33"/>
       <c r="K71" s="96"/>
       <c r="L71" s="108" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M71" s="102" t="s">
-        <v>315</v>
+        <v>249</v>
       </c>
       <c r="N71" s="110" t="s">
         <v>247</v>
@@ -6589,9 +6601,7 @@
       <c r="T71" s="107"/>
     </row>
     <row r="72" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="32" t="s">
-        <v>200</v>
-      </c>
+      <c r="B72" s="32"/>
       <c r="C72" s="33"/>
       <c r="D72" s="33"/>
       <c r="E72" s="33"/>
@@ -6602,7 +6612,7 @@
       <c r="J72" s="33"/>
       <c r="K72" s="96"/>
       <c r="L72" s="108" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="M72" s="102" t="s">
         <v>315</v>
@@ -6619,14 +6629,10 @@
     </row>
     <row r="73" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="C73" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="D73" s="33" t="s">
-        <v>222</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="C73" s="33"/>
+      <c r="D73" s="33"/>
       <c r="E73" s="33"/>
       <c r="F73" s="33"/>
       <c r="G73" s="33"/>
@@ -6635,7 +6641,7 @@
       <c r="J73" s="33"/>
       <c r="K73" s="96"/>
       <c r="L73" s="108" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M73" s="102" t="s">
         <v>315</v>
@@ -6652,13 +6658,13 @@
     </row>
     <row r="74" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="32" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="C74" s="33" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="D74" s="33" t="s">
-        <v>267</v>
+        <v>222</v>
       </c>
       <c r="E74" s="33"/>
       <c r="F74" s="33"/>
@@ -6667,9 +6673,15 @@
       <c r="I74" s="30"/>
       <c r="J74" s="33"/>
       <c r="K74" s="96"/>
-      <c r="L74" s="108"/>
-      <c r="M74" s="102"/>
-      <c r="N74" s="102"/>
+      <c r="L74" s="108" t="s">
+        <v>317</v>
+      </c>
+      <c r="M74" s="102" t="s">
+        <v>315</v>
+      </c>
+      <c r="N74" s="110" t="s">
+        <v>247</v>
+      </c>
       <c r="O74" s="102"/>
       <c r="P74" s="102"/>
       <c r="Q74" s="102"/>
@@ -6678,25 +6690,23 @@
       <c r="T74" s="107"/>
     </row>
     <row r="75" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="80" t="s">
-        <v>268</v>
-      </c>
-      <c r="C75" s="81" t="s">
-        <v>269</v>
-      </c>
-      <c r="D75" s="81" t="s">
-        <v>270</v>
-      </c>
-      <c r="E75" s="81"/>
-      <c r="F75" s="81"/>
-      <c r="G75" s="81"/>
-      <c r="H75" s="81"/>
-      <c r="I75" s="82"/>
-      <c r="J75" s="27"/>
+      <c r="B75" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="C75" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="D75" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="E75" s="33"/>
+      <c r="F75" s="33"/>
+      <c r="G75" s="33"/>
+      <c r="H75" s="33"/>
+      <c r="I75" s="30"/>
+      <c r="J75" s="33"/>
       <c r="K75" s="96"/>
-      <c r="L75" s="108" t="s">
-        <v>200</v>
-      </c>
+      <c r="L75" s="108"/>
       <c r="M75" s="102"/>
       <c r="N75" s="102"/>
       <c r="O75" s="102"/>
@@ -6707,31 +6717,27 @@
       <c r="T75" s="107"/>
     </row>
     <row r="76" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="C76" s="33" t="s">
-        <v>271</v>
-      </c>
-      <c r="D76" s="33" t="s">
-        <v>271</v>
-      </c>
-      <c r="E76" s="33"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="33"/>
-      <c r="H76" s="33"/>
-      <c r="I76" s="30"/>
+      <c r="B76" s="80" t="s">
+        <v>268</v>
+      </c>
+      <c r="C76" s="81" t="s">
+        <v>269</v>
+      </c>
+      <c r="D76" s="81" t="s">
+        <v>270</v>
+      </c>
+      <c r="E76" s="81"/>
+      <c r="F76" s="81"/>
+      <c r="G76" s="81"/>
+      <c r="H76" s="81"/>
+      <c r="I76" s="82"/>
       <c r="J76" s="27"/>
       <c r="K76" s="96"/>
       <c r="L76" s="108" t="s">
-        <v>220</v>
-      </c>
-      <c r="M76" s="102" t="s">
-        <v>221</v>
-      </c>
-      <c r="N76" s="102" t="s">
-        <v>302</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="M76" s="102"/>
+      <c r="N76" s="102"/>
       <c r="O76" s="102"/>
       <c r="P76" s="102"/>
       <c r="Q76" s="102"/>
@@ -6741,13 +6747,13 @@
     </row>
     <row r="77" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="32" t="s">
-        <v>272</v>
+        <v>204</v>
       </c>
       <c r="C77" s="33" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D77" s="33" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E77" s="33"/>
       <c r="F77" s="33"/>
@@ -6757,13 +6763,13 @@
       <c r="J77" s="27"/>
       <c r="K77" s="96"/>
       <c r="L77" s="108" t="s">
-        <v>268</v>
+        <v>220</v>
       </c>
       <c r="M77" s="102" t="s">
-        <v>318</v>
-      </c>
-      <c r="N77" s="110" t="s">
-        <v>319</v>
+        <v>221</v>
+      </c>
+      <c r="N77" s="102" t="s">
+        <v>302</v>
       </c>
       <c r="O77" s="102"/>
       <c r="P77" s="102"/>
@@ -6774,13 +6780,13 @@
     </row>
     <row r="78" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="32" t="s">
-        <v>210</v>
+        <v>272</v>
       </c>
       <c r="C78" s="33" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D78" s="33" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="E78" s="33"/>
       <c r="F78" s="33"/>
@@ -6790,13 +6796,13 @@
       <c r="J78" s="27"/>
       <c r="K78" s="96"/>
       <c r="L78" s="108" t="s">
-        <v>204</v>
+        <v>268</v>
       </c>
       <c r="M78" s="102" t="s">
-        <v>320</v>
-      </c>
-      <c r="N78" s="102" t="s">
-        <v>320</v>
+        <v>318</v>
+      </c>
+      <c r="N78" s="110" t="s">
+        <v>319</v>
       </c>
       <c r="O78" s="102"/>
       <c r="P78" s="102"/>
@@ -6807,13 +6813,13 @@
     </row>
     <row r="79" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="32" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C79" s="33" t="s">
-        <v>207</v>
+        <v>275</v>
       </c>
       <c r="D79" s="33" t="s">
-        <v>207</v>
+        <v>270</v>
       </c>
       <c r="E79" s="33"/>
       <c r="F79" s="33"/>
@@ -6823,7 +6829,7 @@
       <c r="J79" s="27"/>
       <c r="K79" s="96"/>
       <c r="L79" s="108" t="s">
-        <v>272</v>
+        <v>204</v>
       </c>
       <c r="M79" s="102" t="s">
         <v>320</v>
@@ -6840,13 +6846,13 @@
     </row>
     <row r="80" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="32" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C80" s="33" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D80" s="33" t="s">
-        <v>276</v>
+        <v>207</v>
       </c>
       <c r="E80" s="33"/>
       <c r="F80" s="33"/>
@@ -6856,13 +6862,13 @@
       <c r="J80" s="27"/>
       <c r="K80" s="96"/>
       <c r="L80" s="108" t="s">
-        <v>210</v>
+        <v>272</v>
       </c>
       <c r="M80" s="102" t="s">
-        <v>321</v>
-      </c>
-      <c r="N80" s="110" t="s">
-        <v>322</v>
+        <v>320</v>
+      </c>
+      <c r="N80" s="102" t="s">
+        <v>320</v>
       </c>
       <c r="O80" s="102"/>
       <c r="P80" s="102"/>
@@ -6873,13 +6879,13 @@
     </row>
     <row r="81" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="32" t="s">
-        <v>277</v>
+        <v>212</v>
       </c>
       <c r="C81" s="33" t="s">
-        <v>273</v>
+        <v>211</v>
       </c>
       <c r="D81" s="33" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="E81" s="33"/>
       <c r="F81" s="33"/>
@@ -6889,13 +6895,13 @@
       <c r="J81" s="27"/>
       <c r="K81" s="96"/>
       <c r="L81" s="108" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="M81" s="102" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="N81" s="110" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="O81" s="102"/>
       <c r="P81" s="102"/>
@@ -6905,9 +6911,15 @@
       <c r="T81" s="107"/>
     </row>
     <row r="82" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="32"/>
-      <c r="C82" s="33"/>
-      <c r="D82" s="33"/>
+      <c r="B82" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="C82" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="D82" s="33" t="s">
+        <v>274</v>
+      </c>
       <c r="E82" s="33"/>
       <c r="F82" s="33"/>
       <c r="G82" s="33"/>
@@ -6916,13 +6928,13 @@
       <c r="J82" s="27"/>
       <c r="K82" s="96"/>
       <c r="L82" s="108" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="M82" s="102" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="N82" s="110" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="O82" s="102"/>
       <c r="P82" s="102"/>
@@ -6932,9 +6944,7 @@
       <c r="T82" s="107"/>
     </row>
     <row r="83" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="32" t="s">
-        <v>213</v>
-      </c>
+      <c r="B83" s="32"/>
       <c r="C83" s="33"/>
       <c r="D83" s="33"/>
       <c r="E83" s="33"/>
@@ -6945,13 +6955,13 @@
       <c r="J83" s="27"/>
       <c r="K83" s="96"/>
       <c r="L83" s="108" t="s">
-        <v>277</v>
+        <v>212</v>
       </c>
       <c r="M83" s="102" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N83" s="110" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="O83" s="102"/>
       <c r="P83" s="102"/>
@@ -6962,55 +6972,58 @@
     </row>
     <row r="84" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="C84" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="D84" s="33" t="s">
-        <v>222</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="C84" s="33"/>
+      <c r="D84" s="33"/>
       <c r="E84" s="33"/>
       <c r="F84" s="33"/>
       <c r="G84" s="33"/>
       <c r="H84" s="33"/>
       <c r="I84" s="30"/>
       <c r="J84" s="27"/>
-      <c r="L84" s="60" t="s">
+      <c r="K84" s="96"/>
+      <c r="L84" s="108" t="s">
+        <v>277</v>
+      </c>
+      <c r="M84" s="102" t="s">
+        <v>326</v>
+      </c>
+      <c r="N84" s="110" t="s">
+        <v>326</v>
+      </c>
+      <c r="O84" s="102"/>
+      <c r="P84" s="102"/>
+      <c r="Q84" s="102"/>
+      <c r="R84" s="102"/>
+      <c r="S84" s="109"/>
+      <c r="T84" s="107"/>
+    </row>
+    <row r="85" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="C85" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="D85" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="E85" s="33"/>
+      <c r="F85" s="33"/>
+      <c r="G85" s="33"/>
+      <c r="H85" s="33"/>
+      <c r="I85" s="30"/>
+      <c r="J85" s="27"/>
+      <c r="L85" s="60" t="s">
         <v>327</v>
       </c>
-      <c r="M84" s="57" t="s">
+      <c r="M85" s="57" t="s">
         <v>328</v>
       </c>
-      <c r="N84" s="58" t="s">
+      <c r="N85" s="58" t="s">
         <v>329</v>
       </c>
-      <c r="O84" s="57"/>
-      <c r="P84" s="57"/>
-      <c r="Q84" s="57"/>
-      <c r="R84" s="57"/>
-      <c r="S84" s="62"/>
-      <c r="T84" s="61"/>
-    </row>
-    <row r="85" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="80" t="s">
-        <v>278</v>
-      </c>
-      <c r="C85" s="81" t="s">
-        <v>279</v>
-      </c>
-      <c r="D85" s="81" t="s">
-        <v>280</v>
-      </c>
-      <c r="E85" s="81"/>
-      <c r="F85" s="81"/>
-      <c r="G85" s="81"/>
-      <c r="H85" s="81"/>
-      <c r="I85" s="82"/>
-      <c r="J85" s="27"/>
-      <c r="L85" s="60"/>
-      <c r="M85" s="57"/>
-      <c r="N85" s="57"/>
       <c r="O85" s="57"/>
       <c r="P85" s="57"/>
       <c r="Q85" s="57"/>
@@ -7020,13 +7033,13 @@
     </row>
     <row r="86" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="80" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C86" s="81" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D86" s="81" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E86" s="81"/>
       <c r="F86" s="81"/>
@@ -7034,9 +7047,7 @@
       <c r="H86" s="81"/>
       <c r="I86" s="82"/>
       <c r="J86" s="27"/>
-      <c r="L86" s="60" t="s">
-        <v>213</v>
-      </c>
+      <c r="L86" s="60"/>
       <c r="M86" s="57"/>
       <c r="N86" s="57"/>
       <c r="O86" s="57"/>
@@ -7047,30 +7058,26 @@
       <c r="T86" s="61"/>
     </row>
     <row r="87" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="32" t="s">
-        <v>215</v>
-      </c>
-      <c r="C87" s="33" t="s">
-        <v>284</v>
-      </c>
-      <c r="D87" s="33" t="s">
-        <v>285</v>
-      </c>
-      <c r="E87" s="33"/>
-      <c r="F87" s="33"/>
-      <c r="G87" s="33"/>
-      <c r="H87" s="33"/>
-      <c r="I87" s="30"/>
+      <c r="B87" s="80" t="s">
+        <v>281</v>
+      </c>
+      <c r="C87" s="81" t="s">
+        <v>282</v>
+      </c>
+      <c r="D87" s="81" t="s">
+        <v>283</v>
+      </c>
+      <c r="E87" s="81"/>
+      <c r="F87" s="81"/>
+      <c r="G87" s="81"/>
+      <c r="H87" s="81"/>
+      <c r="I87" s="82"/>
       <c r="J87" s="27"/>
       <c r="L87" s="60" t="s">
-        <v>220</v>
-      </c>
-      <c r="M87" s="57" t="s">
-        <v>221</v>
-      </c>
-      <c r="N87" s="57" t="s">
-        <v>302</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="M87" s="57"/>
+      <c r="N87" s="57"/>
       <c r="O87" s="57"/>
       <c r="P87" s="57"/>
       <c r="Q87" s="57"/>
@@ -7079,61 +7086,61 @@
       <c r="T87" s="61"/>
     </row>
     <row r="88" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="80" t="s">
+      <c r="B88" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="C88" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="D88" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="E88" s="33"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="33"/>
+      <c r="H88" s="33"/>
+      <c r="I88" s="30"/>
+      <c r="J88" s="27"/>
+      <c r="L88" s="60" t="s">
+        <v>220</v>
+      </c>
+      <c r="M88" s="57" t="s">
+        <v>221</v>
+      </c>
+      <c r="N88" s="57" t="s">
+        <v>302</v>
+      </c>
+      <c r="O88" s="57"/>
+      <c r="P88" s="57"/>
+      <c r="Q88" s="57"/>
+      <c r="R88" s="57"/>
+      <c r="S88" s="62"/>
+      <c r="T88" s="61"/>
+    </row>
+    <row r="89" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="80" t="s">
         <v>286</v>
       </c>
-      <c r="C88" s="81" t="s">
+      <c r="C89" s="81" t="s">
         <v>287</v>
       </c>
-      <c r="D88" s="81" t="s">
+      <c r="D89" s="81" t="s">
         <v>288</v>
       </c>
-      <c r="E88" s="81"/>
-      <c r="F88" s="81"/>
-      <c r="G88" s="81"/>
-      <c r="H88" s="81"/>
-      <c r="I88" s="82"/>
-      <c r="J88" s="27"/>
-      <c r="L88" s="83" t="s">
-        <v>278</v>
-      </c>
-      <c r="M88" s="84" t="s">
-        <v>282</v>
-      </c>
-      <c r="N88" s="85" t="s">
-        <v>283</v>
-      </c>
-      <c r="O88" s="84"/>
-      <c r="P88" s="84"/>
-      <c r="Q88" s="84"/>
-      <c r="R88" s="84"/>
-      <c r="S88" s="86"/>
-      <c r="T88" s="61"/>
-    </row>
-    <row r="89" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="32" t="s">
-        <v>218</v>
-      </c>
-      <c r="C89" s="33" t="s">
-        <v>289</v>
-      </c>
-      <c r="D89" s="33" t="s">
-        <v>290</v>
-      </c>
-      <c r="E89" s="33"/>
-      <c r="F89" s="33"/>
-      <c r="G89" s="33"/>
-      <c r="H89" s="33"/>
-      <c r="I89" s="30"/>
+      <c r="E89" s="81"/>
+      <c r="F89" s="81"/>
+      <c r="G89" s="81"/>
+      <c r="H89" s="81"/>
+      <c r="I89" s="82"/>
       <c r="J89" s="27"/>
       <c r="L89" s="83" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="M89" s="84" t="s">
-        <v>330</v>
+        <v>282</v>
       </c>
       <c r="N89" s="85" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="O89" s="84"/>
       <c r="P89" s="84"/>
@@ -7143,26 +7150,26 @@
       <c r="T89" s="61"/>
     </row>
     <row r="90" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="80" t="s">
-        <v>291</v>
-      </c>
-      <c r="C90" s="81" t="s">
-        <v>292</v>
-      </c>
-      <c r="D90" s="81" t="s">
-        <v>292</v>
-      </c>
-      <c r="E90" s="81"/>
-      <c r="F90" s="81"/>
-      <c r="G90" s="81"/>
-      <c r="H90" s="81"/>
-      <c r="I90" s="82"/>
+      <c r="B90" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="C90" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="D90" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="E90" s="33"/>
+      <c r="F90" s="33"/>
+      <c r="G90" s="33"/>
+      <c r="H90" s="33"/>
+      <c r="I90" s="30"/>
       <c r="J90" s="27"/>
       <c r="L90" s="83" t="s">
-        <v>215</v>
+        <v>281</v>
       </c>
       <c r="M90" s="84" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N90" s="85" t="s">
         <v>280</v>
@@ -7175,72 +7182,104 @@
       <c r="T90" s="61"/>
     </row>
     <row r="91" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="59" t="s">
+      <c r="B91" s="80" t="s">
+        <v>291</v>
+      </c>
+      <c r="C91" s="81" t="s">
+        <v>292</v>
+      </c>
+      <c r="D91" s="81" t="s">
+        <v>292</v>
+      </c>
+      <c r="E91" s="81"/>
+      <c r="F91" s="81"/>
+      <c r="G91" s="81"/>
+      <c r="H91" s="81"/>
+      <c r="I91" s="82"/>
+      <c r="J91" s="27"/>
+      <c r="L91" s="83" t="s">
+        <v>215</v>
+      </c>
+      <c r="M91" s="84" t="s">
+        <v>331</v>
+      </c>
+      <c r="N91" s="85" t="s">
+        <v>280</v>
+      </c>
+      <c r="O91" s="84"/>
+      <c r="P91" s="84"/>
+      <c r="Q91" s="84"/>
+      <c r="R91" s="84"/>
+      <c r="S91" s="86"/>
+      <c r="T91" s="61"/>
+    </row>
+    <row r="92" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="59" t="s">
         <v>219</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C92" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="D91" s="13" t="s">
+      <c r="D92" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="E91" s="13"/>
-      <c r="F91" s="13"/>
-      <c r="G91" s="13"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="31"/>
-      <c r="J91" s="27"/>
-      <c r="L91" s="60" t="s">
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="31"/>
+      <c r="J92" s="27"/>
+      <c r="L92" s="60" t="s">
         <v>286</v>
       </c>
-      <c r="M91" s="57" t="s">
+      <c r="M92" s="57" t="s">
         <v>332</v>
       </c>
-      <c r="N91" s="58" t="s">
+      <c r="N92" s="58" t="s">
         <v>333</v>
       </c>
-      <c r="O91" s="57"/>
-      <c r="P91" s="57"/>
-      <c r="Q91" s="57"/>
-      <c r="R91" s="57"/>
-      <c r="S91" s="62"/>
-      <c r="T91" s="61"/>
-    </row>
-    <row r="92" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L92" s="63" t="s">
+      <c r="O92" s="57"/>
+      <c r="P92" s="57"/>
+      <c r="Q92" s="57"/>
+      <c r="R92" s="57"/>
+      <c r="S92" s="62"/>
+      <c r="T92" s="61"/>
+    </row>
+    <row r="93" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L93" s="63" t="s">
         <v>219</v>
       </c>
-      <c r="M92" s="64" t="s">
+      <c r="M93" s="64" t="s">
         <v>334</v>
       </c>
-      <c r="N92" s="65" t="s">
+      <c r="N93" s="65" t="s">
         <v>294</v>
       </c>
-      <c r="O92" s="64"/>
-      <c r="P92" s="64"/>
-      <c r="Q92" s="64"/>
-      <c r="R92" s="64"/>
-      <c r="S92" s="66"/>
-      <c r="T92" s="61"/>
+      <c r="O93" s="64"/>
+      <c r="P93" s="64"/>
+      <c r="Q93" s="64"/>
+      <c r="R93" s="64"/>
+      <c r="S93" s="66"/>
+      <c r="T93" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="L33:S33"/>
+    <mergeCell ref="L34:S34"/>
     <mergeCell ref="L15:L19"/>
     <mergeCell ref="L20:L26"/>
-    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="L27:L29"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="L4:P5"/>
     <mergeCell ref="L7:L14"/>
     <mergeCell ref="V4:Z5"/>
-    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="B34:I34"/>
     <mergeCell ref="A1:F3"/>
-    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A30:A32"/>
     <mergeCell ref="A4:E5"/>
     <mergeCell ref="A7:A14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A23:A29"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I4:J4"/>

</xml_diff>

<commit_message>
3/15: no atmega32u4-MU yet
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Hydration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265C1FF9-6A58-4487-92DF-ABFF42B94B26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AF3F1A-4EDC-4DCD-B1A9-BF176B1DD426}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{C3AD9D2E-3E69-485C-A23B-91E4490D16E1}"/>
   </bookViews>
@@ -1251,7 +1251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1339,6 +1339,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1946,7 +1952,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="211">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2327,20 +2333,101 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2423,87 +2510,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2851,12 +2862,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="156" t="s">
+      <c r="B1" s="152" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
       <c r="I1" s="69"/>
       <c r="J1" s="69"/>
       <c r="K1" s="69"/>
@@ -2890,7 +2901,7 @@
       <c r="M2" s="69"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="153" t="s">
+      <c r="A3" s="155" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -2918,7 +2929,7 @@
       <c r="M3" s="69"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="154"/>
+      <c r="A4" s="156"/>
       <c r="B4" s="4" t="s">
         <v>95</v>
       </c>
@@ -2941,7 +2952,7 @@
       <c r="M4" s="69"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="154"/>
+      <c r="A5" s="156"/>
       <c r="B5" s="6" t="s">
         <v>127</v>
       </c>
@@ -2974,7 +2985,7 @@
       <c r="M6" s="69"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="152" t="s">
+      <c r="A7" s="153" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
@@ -2999,7 +3010,7 @@
       <c r="M7" s="69"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="152"/>
+      <c r="A8" s="153"/>
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -3022,7 +3033,7 @@
       <c r="M8" s="69"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="152"/>
+      <c r="A9" s="153"/>
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -3045,7 +3056,7 @@
       <c r="M9" s="69"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="152"/>
+      <c r="A10" s="153"/>
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -3068,7 +3079,7 @@
       <c r="M10" s="69"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="152"/>
+      <c r="A11" s="153"/>
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -3091,7 +3102,7 @@
       <c r="M11" s="69"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="152"/>
+      <c r="A12" s="153"/>
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -3153,7 +3164,7 @@
       <c r="M15" s="69"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="152" t="s">
+      <c r="A16" s="153" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -3176,7 +3187,7 @@
       <c r="M16" s="69"/>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="152"/>
+      <c r="A17" s="153"/>
       <c r="B17" s="4" t="s">
         <v>22</v>
       </c>
@@ -3196,7 +3207,7 @@
       <c r="M17" s="69"/>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="152"/>
+      <c r="A18" s="153"/>
       <c r="B18" s="4" t="s">
         <v>24</v>
       </c>
@@ -3216,7 +3227,7 @@
       <c r="M18" s="69"/>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="152"/>
+      <c r="A19" s="153"/>
       <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
@@ -3237,7 +3248,7 @@
       <c r="M19" s="69"/>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="152"/>
+      <c r="A20" s="153"/>
       <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
@@ -3258,7 +3269,7 @@
       <c r="M20" s="69"/>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="152"/>
+      <c r="A21" s="153"/>
       <c r="B21" s="4" t="s">
         <v>30</v>
       </c>
@@ -3278,7 +3289,7 @@
       <c r="M21" s="69"/>
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="152"/>
+      <c r="A22" s="153"/>
       <c r="B22" s="4" t="s">
         <v>32</v>
       </c>
@@ -3299,7 +3310,7 @@
       <c r="M22" s="69"/>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="152"/>
+      <c r="A23" s="153"/>
       <c r="B23" s="4" t="s">
         <v>34</v>
       </c>
@@ -3320,7 +3331,7 @@
       <c r="M23" s="69"/>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="152"/>
+      <c r="A24" s="153"/>
       <c r="B24" s="4" t="s">
         <v>38</v>
       </c>
@@ -3340,7 +3351,7 @@
       <c r="M24" s="69"/>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="152"/>
+      <c r="A25" s="153"/>
       <c r="B25" s="4" t="s">
         <v>40</v>
       </c>
@@ -3360,7 +3371,7 @@
       <c r="M25" s="69"/>
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="152"/>
+      <c r="A26" s="153"/>
       <c r="B26" s="4" t="s">
         <v>42</v>
       </c>
@@ -3380,7 +3391,7 @@
       <c r="M26" s="69"/>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="152"/>
+      <c r="A27" s="153"/>
       <c r="B27" s="4" t="s">
         <v>45</v>
       </c>
@@ -3407,7 +3418,7 @@
       <c r="M28" s="69"/>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="152" t="s">
+      <c r="A29" s="153" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -3430,7 +3441,7 @@
       <c r="M29" s="69"/>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="152"/>
+      <c r="A30" s="153"/>
       <c r="B30" s="4" t="s">
         <v>47</v>
       </c>
@@ -3450,7 +3461,7 @@
       <c r="M30" s="69"/>
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="152"/>
+      <c r="A31" s="153"/>
       <c r="B31" s="4" t="s">
         <v>44</v>
       </c>
@@ -3470,7 +3481,7 @@
       <c r="M31" s="69"/>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="152"/>
+      <c r="A32" s="153"/>
       <c r="B32" s="4" t="s">
         <v>50</v>
       </c>
@@ -3490,7 +3501,7 @@
       <c r="M32" s="69"/>
     </row>
     <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="152"/>
+      <c r="A33" s="153"/>
       <c r="B33" s="4" t="s">
         <v>53</v>
       </c>
@@ -3510,7 +3521,7 @@
       <c r="M33" s="69"/>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="152"/>
+      <c r="A34" s="153"/>
       <c r="B34" s="4" t="s">
         <v>55</v>
       </c>
@@ -3533,7 +3544,7 @@
       <c r="M34" s="69"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="152" t="s">
+      <c r="A36" s="153" t="s">
         <v>58</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -3550,7 +3561,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="152"/>
+      <c r="A37" s="153"/>
       <c r="B37" s="4" t="s">
         <v>61</v>
       </c>
@@ -3565,7 +3576,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="152" t="s">
+      <c r="A39" s="153" t="s">
         <v>63</v>
       </c>
       <c r="B39" s="8" t="s">
@@ -3588,7 +3599,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="152"/>
+      <c r="A40" s="153"/>
       <c r="B40" t="s">
         <v>65</v>
       </c>
@@ -3606,7 +3617,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="152"/>
+      <c r="A41" s="153"/>
       <c r="B41" s="4" t="s">
         <v>84</v>
       </c>
@@ -3624,7 +3635,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="152"/>
+      <c r="A42" s="153"/>
       <c r="B42" s="4" t="s">
         <v>101</v>
       </c>
@@ -3659,7 +3670,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="155" t="s">
+      <c r="A45" s="154" t="s">
         <v>72</v>
       </c>
       <c r="B45" s="8" t="s">
@@ -3679,7 +3690,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="155"/>
+      <c r="A46" s="154"/>
       <c r="B46" s="4" t="s">
         <v>80</v>
       </c>
@@ -3701,7 +3712,7 @@
       <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="155" t="s">
+      <c r="A48" s="154" t="s">
         <v>106</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -3718,7 +3729,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="155"/>
+      <c r="A49" s="154"/>
       <c r="B49" s="4" t="s">
         <v>140</v>
       </c>
@@ -3730,7 +3741,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="152" t="s">
+      <c r="A51" s="153" t="s">
         <v>69</v>
       </c>
       <c r="B51" t="s">
@@ -3750,7 +3761,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="152"/>
+      <c r="A52" s="153"/>
       <c r="B52" s="4" t="s">
         <v>73</v>
       </c>
@@ -3765,7 +3776,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="152"/>
+      <c r="A53" s="153"/>
       <c r="B53" s="4" t="s">
         <v>75</v>
       </c>
@@ -3780,7 +3791,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="152"/>
+      <c r="A54" s="153"/>
       <c r="B54" s="4" t="s">
         <v>82</v>
       </c>
@@ -3795,7 +3806,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="152"/>
+      <c r="A55" s="153"/>
       <c r="B55" s="37" t="s">
         <v>88</v>
       </c>
@@ -3813,7 +3824,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="152"/>
+      <c r="A56" s="153"/>
       <c r="B56" s="4" t="s">
         <v>91</v>
       </c>
@@ -3828,7 +3839,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="152"/>
+      <c r="A57" s="153"/>
       <c r="B57" s="4" t="s">
         <v>93</v>
       </c>
@@ -3843,7 +3854,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="152"/>
+      <c r="A58" s="153"/>
       <c r="B58" s="4" t="s">
         <v>109</v>
       </c>
@@ -3858,7 +3869,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="152"/>
+      <c r="A59" s="153"/>
       <c r="B59" s="4" t="s">
         <v>111</v>
       </c>
@@ -3873,7 +3884,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="152"/>
+      <c r="A60" s="153"/>
       <c r="B60" s="8" t="s">
         <v>113</v>
       </c>
@@ -3888,7 +3899,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="152"/>
+      <c r="A61" s="153"/>
       <c r="B61" s="4" t="s">
         <v>118</v>
       </c>
@@ -3906,7 +3917,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="152"/>
+      <c r="A62" s="153"/>
       <c r="B62" s="37" t="s">
         <v>121</v>
       </c>
@@ -3924,7 +3935,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="152"/>
+      <c r="A63" s="153"/>
       <c r="B63" s="4" t="s">
         <v>123</v>
       </c>
@@ -3942,7 +3953,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="152"/>
+      <c r="A64" s="153"/>
       <c r="B64" s="4" t="s">
         <v>130</v>
       </c>
@@ -3960,7 +3971,7 @@
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="152"/>
+      <c r="A65" s="153"/>
       <c r="B65" s="4" t="s">
         <v>133</v>
       </c>
@@ -3978,7 +3989,7 @@
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="152"/>
+      <c r="A66" s="153"/>
       <c r="B66" s="4" t="s">
         <v>136</v>
       </c>
@@ -3993,7 +4004,7 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="152"/>
+      <c r="A67" s="153"/>
       <c r="B67" s="4" t="s">
         <v>142</v>
       </c>
@@ -4008,7 +4019,7 @@
       </c>
     </row>
     <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="152"/>
+      <c r="A68" s="153"/>
       <c r="B68" s="8" t="s">
         <v>145</v>
       </c>
@@ -4023,7 +4034,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="152" t="s">
+      <c r="A70" s="153" t="s">
         <v>116</v>
       </c>
       <c r="B70" s="4" t="s">
@@ -4043,7 +4054,7 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="152"/>
+      <c r="A71" s="153"/>
       <c r="B71" s="4" t="s">
         <v>102</v>
       </c>
@@ -4055,7 +4066,7 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="152"/>
+      <c r="A72" s="153"/>
       <c r="B72" s="4" t="s">
         <v>115</v>
       </c>
@@ -4071,7 +4082,7 @@
       <c r="H73" s="25"/>
     </row>
     <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="152" t="s">
+      <c r="A74" s="153" t="s">
         <v>148</v>
       </c>
       <c r="B74" s="15" t="s">
@@ -4092,7 +4103,7 @@
       <c r="K74" s="25"/>
     </row>
     <row r="75" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A75" s="152"/>
+      <c r="A75" s="153"/>
       <c r="B75" s="16">
         <v>2601151022113</v>
       </c>
@@ -4107,7 +4118,7 @@
       </c>
     </row>
     <row r="76" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="152"/>
+      <c r="A76" s="153"/>
       <c r="B76" s="16">
         <v>261151044113</v>
       </c>
@@ -4122,7 +4133,7 @@
       </c>
     </row>
     <row r="77" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="152"/>
+      <c r="A77" s="153"/>
       <c r="B77" s="16">
         <v>20012107818</v>
       </c>
@@ -4137,7 +4148,7 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="152"/>
+      <c r="A78" s="153"/>
       <c r="B78" s="16" t="s">
         <v>155</v>
       </c>
@@ -4152,7 +4163,7 @@
       </c>
     </row>
     <row r="79" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="152"/>
+      <c r="A79" s="153"/>
       <c r="B79" s="17">
         <v>260151022110</v>
       </c>
@@ -4167,7 +4178,7 @@
       </c>
     </row>
     <row r="80" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="152"/>
+      <c r="A80" s="153"/>
       <c r="B80" s="16">
         <v>260121011717</v>
       </c>
@@ -4182,7 +4193,7 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="152"/>
+      <c r="A81" s="153"/>
       <c r="B81" s="16">
         <v>20012104412</v>
       </c>
@@ -4198,11 +4209,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A45:A46"/>
     <mergeCell ref="A74:A81"/>
     <mergeCell ref="A70:A72"/>
     <mergeCell ref="A3:A5"/>
@@ -4210,6 +4216,11 @@
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="A51:A68"/>
     <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A45:A46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -4221,7 +4232,7 @@
   <dimension ref="A1:AD93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E7"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4239,106 +4250,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="160" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="189"/>
-      <c r="H1" s="208" t="s">
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
+      <c r="H1" s="181" t="s">
         <v>369</v>
       </c>
-      <c r="I1" s="209"/>
-      <c r="J1" s="210"/>
+      <c r="I1" s="182"/>
+      <c r="J1" s="183"/>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:29" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="190"/>
-      <c r="B2" s="191"/>
-      <c r="C2" s="191"/>
-      <c r="D2" s="191"/>
-      <c r="E2" s="191"/>
-      <c r="F2" s="192"/>
+      <c r="A2" s="163"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="165"/>
       <c r="H2" s="77"/>
-      <c r="I2" s="204" t="s">
+      <c r="I2" s="177" t="s">
         <v>370</v>
       </c>
-      <c r="J2" s="205"/>
+      <c r="J2" s="178"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:29" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="193"/>
-      <c r="B3" s="194"/>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="195"/>
+      <c r="A3" s="166"/>
+      <c r="B3" s="167"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="168"/>
       <c r="H3" s="144"/>
-      <c r="I3" s="204" t="s">
+      <c r="I3" s="177" t="s">
         <v>365</v>
       </c>
-      <c r="J3" s="205"/>
+      <c r="J3" s="178"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="198" t="s">
+      <c r="A4" s="171" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="198"/>
-      <c r="C4" s="198"/>
-      <c r="D4" s="198"/>
-      <c r="E4" s="199"/>
+      <c r="B4" s="171"/>
+      <c r="C4" s="171"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="172"/>
       <c r="F4" s="44"/>
       <c r="G4" s="32"/>
       <c r="H4" s="145"/>
-      <c r="I4" s="206" t="s">
+      <c r="I4" s="179" t="s">
         <v>371</v>
       </c>
-      <c r="J4" s="207"/>
+      <c r="J4" s="180"/>
       <c r="K4" s="143"/>
-      <c r="L4" s="157" t="s">
+      <c r="L4" s="184" t="s">
         <v>357</v>
       </c>
-      <c r="M4" s="158"/>
-      <c r="N4" s="158"/>
-      <c r="O4" s="158"/>
-      <c r="P4" s="159"/>
+      <c r="M4" s="185"/>
+      <c r="N4" s="185"/>
+      <c r="O4" s="185"/>
+      <c r="P4" s="186"/>
       <c r="Q4" s="44"/>
       <c r="R4" s="93"/>
       <c r="U4" s="93"/>
-      <c r="V4" s="166" t="s">
+      <c r="V4" s="193" t="s">
         <v>372</v>
       </c>
-      <c r="W4" s="167"/>
-      <c r="X4" s="167"/>
-      <c r="Y4" s="167"/>
-      <c r="Z4" s="168"/>
+      <c r="W4" s="194"/>
+      <c r="X4" s="194"/>
+      <c r="Y4" s="194"/>
+      <c r="Z4" s="195"/>
       <c r="AA4" s="93"/>
       <c r="AB4" s="32"/>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="200"/>
-      <c r="B5" s="200"/>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="173"/>
+      <c r="C5" s="173"/>
+      <c r="D5" s="173"/>
+      <c r="E5" s="174"/>
       <c r="F5" s="44"/>
       <c r="G5" s="32"/>
-      <c r="L5" s="160"/>
-      <c r="M5" s="161"/>
-      <c r="N5" s="161"/>
-      <c r="O5" s="161"/>
-      <c r="P5" s="162"/>
+      <c r="L5" s="187"/>
+      <c r="M5" s="188"/>
+      <c r="N5" s="188"/>
+      <c r="O5" s="188"/>
+      <c r="P5" s="189"/>
       <c r="Q5" s="44"/>
       <c r="R5" s="93"/>
       <c r="U5" s="93"/>
-      <c r="V5" s="169"/>
-      <c r="W5" s="170"/>
-      <c r="X5" s="170"/>
-      <c r="Y5" s="170"/>
-      <c r="Z5" s="171"/>
+      <c r="V5" s="196"/>
+      <c r="W5" s="197"/>
+      <c r="X5" s="197"/>
+      <c r="Y5" s="197"/>
+      <c r="Z5" s="198"/>
       <c r="AA5" s="93"/>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4394,7 +4405,7 @@
       <c r="AA6" s="93"/>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="196" t="s">
+      <c r="A7" s="169" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="88" t="s">
@@ -4411,7 +4422,7 @@
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="32"/>
-      <c r="L7" s="163" t="s">
+      <c r="L7" s="190" t="s">
         <v>339</v>
       </c>
       <c r="M7" s="88" t="s">
@@ -4450,7 +4461,7 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="196"/>
+      <c r="A8" s="169"/>
       <c r="B8" s="26" t="s">
         <v>167</v>
       </c>
@@ -4467,7 +4478,7 @@
         <v>382</v>
       </c>
       <c r="G8" s="32"/>
-      <c r="L8" s="164"/>
+      <c r="L8" s="191"/>
       <c r="M8" s="26" t="s">
         <v>341</v>
       </c>
@@ -4504,7 +4515,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="196"/>
+      <c r="A9" s="169"/>
       <c r="B9" s="26" t="s">
         <v>169</v>
       </c>
@@ -4521,7 +4532,7 @@
         <v>382</v>
       </c>
       <c r="G9" s="32"/>
-      <c r="L9" s="164"/>
+      <c r="L9" s="191"/>
       <c r="M9" s="70" t="s">
         <v>173</v>
       </c>
@@ -4558,7 +4569,7 @@
       </c>
     </row>
     <row r="10" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="196"/>
+      <c r="A10" s="169"/>
       <c r="B10" s="26" t="s">
         <v>172</v>
       </c>
@@ -4575,7 +4586,7 @@
         <v>382</v>
       </c>
       <c r="G10" s="32"/>
-      <c r="L10" s="164"/>
+      <c r="L10" s="191"/>
       <c r="M10" s="70" t="s">
         <v>178</v>
       </c>
@@ -4610,7 +4621,7 @@
       <c r="AA10" s="93"/>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="196"/>
+      <c r="A11" s="169"/>
       <c r="B11" s="26" t="s">
         <v>173</v>
       </c>
@@ -4626,7 +4637,7 @@
       <c r="F11" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="L11" s="164"/>
+      <c r="L11" s="191"/>
       <c r="M11" s="26" t="s">
         <v>345</v>
       </c>
@@ -4651,7 +4662,7 @@
       <c r="AA11" s="32"/>
     </row>
     <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="196"/>
+      <c r="A12" s="169"/>
       <c r="B12" s="26" t="s">
         <v>176</v>
       </c>
@@ -4667,7 +4678,7 @@
       <c r="F12" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="L12" s="164"/>
+      <c r="L12" s="191"/>
       <c r="M12" s="26" t="s">
         <v>348</v>
       </c>
@@ -4692,7 +4703,7 @@
       <c r="AA12" s="32"/>
     </row>
     <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="196"/>
+      <c r="A13" s="169"/>
       <c r="B13" s="26" t="s">
         <v>178</v>
       </c>
@@ -4708,7 +4719,7 @@
       <c r="F13" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="L13" s="164"/>
+      <c r="L13" s="191"/>
       <c r="M13" s="70" t="s">
         <v>181</v>
       </c>
@@ -4733,7 +4744,7 @@
       <c r="AB13" s="93"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="202"/>
+      <c r="A14" s="175"/>
       <c r="B14" s="91" t="s">
         <v>181</v>
       </c>
@@ -4749,7 +4760,7 @@
       <c r="F14" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="L14" s="165"/>
+      <c r="L14" s="192"/>
       <c r="M14" s="91" t="s">
         <v>350</v>
       </c>
@@ -4775,7 +4786,7 @@
       <c r="AC14" s="93"/>
     </row>
     <row r="15" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="203" t="s">
+      <c r="A15" s="176" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="92" t="s">
@@ -4793,7 +4804,7 @@
       <c r="F15" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="L15" s="178" t="s">
+      <c r="L15" s="205" t="s">
         <v>36</v>
       </c>
       <c r="M15" s="112" t="s">
@@ -4811,19 +4822,19 @@
       <c r="Q15" s="44" t="s">
         <v>382</v>
       </c>
-      <c r="V15" s="172" t="s">
+      <c r="V15" s="199" t="s">
         <v>337</v>
       </c>
-      <c r="W15" s="173"/>
-      <c r="X15" s="173"/>
-      <c r="Y15" s="173"/>
-      <c r="Z15" s="173"/>
-      <c r="AA15" s="173"/>
-      <c r="AB15" s="173"/>
-      <c r="AC15" s="174"/>
+      <c r="W15" s="200"/>
+      <c r="X15" s="200"/>
+      <c r="Y15" s="200"/>
+      <c r="Z15" s="200"/>
+      <c r="AA15" s="200"/>
+      <c r="AB15" s="200"/>
+      <c r="AC15" s="201"/>
     </row>
     <row r="16" spans="1:29" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="196"/>
+      <c r="A16" s="169"/>
       <c r="B16" s="26" t="s">
         <v>183</v>
       </c>
@@ -4839,7 +4850,7 @@
       <c r="F16" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="L16" s="179"/>
+      <c r="L16" s="206"/>
       <c r="M16" s="70" t="s">
         <v>183</v>
       </c>
@@ -4868,7 +4879,7 @@
       <c r="AC16" s="146"/>
     </row>
     <row r="17" spans="1:30" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="202"/>
+      <c r="A17" s="175"/>
       <c r="B17" s="91" t="s">
         <v>185</v>
       </c>
@@ -4884,7 +4895,7 @@
       <c r="F17" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="L17" s="179"/>
+      <c r="L17" s="206"/>
       <c r="M17" s="70" t="s">
         <v>185</v>
       </c>
@@ -4916,7 +4927,7 @@
       <c r="AC17" s="103"/>
     </row>
     <row r="18" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="203" t="s">
+      <c r="A18" s="176" t="s">
         <v>199</v>
       </c>
       <c r="B18" s="26" t="s">
@@ -4932,7 +4943,7 @@
         <v>190</v>
       </c>
       <c r="F18" s="14"/>
-      <c r="L18" s="179"/>
+      <c r="L18" s="206"/>
       <c r="M18" s="26" t="s">
         <v>355</v>
       </c>
@@ -4964,7 +4975,7 @@
       <c r="AC18" s="106"/>
     </row>
     <row r="19" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="196"/>
+      <c r="A19" s="169"/>
       <c r="B19" s="26" t="s">
         <v>191</v>
       </c>
@@ -4978,7 +4989,7 @@
         <v>192</v>
       </c>
       <c r="F19" s="131"/>
-      <c r="L19" s="180"/>
+      <c r="L19" s="207"/>
       <c r="M19" s="91" t="s">
         <v>356</v>
       </c>
@@ -5010,7 +5021,7 @@
       <c r="AC19" s="106"/>
     </row>
     <row r="20" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="196"/>
+      <c r="A20" s="169"/>
       <c r="B20" s="26" t="s">
         <v>193</v>
       </c>
@@ -5024,7 +5035,7 @@
         <v>194</v>
       </c>
       <c r="F20" s="131"/>
-      <c r="L20" s="178" t="s">
+      <c r="L20" s="205" t="s">
         <v>200</v>
       </c>
       <c r="M20" s="109" t="s">
@@ -5050,7 +5061,7 @@
       <c r="AC20" s="106"/>
     </row>
     <row r="21" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="196"/>
+      <c r="A21" s="169"/>
       <c r="B21" s="26" t="s">
         <v>195</v>
       </c>
@@ -5064,7 +5075,7 @@
         <v>196</v>
       </c>
       <c r="F21" s="131"/>
-      <c r="L21" s="179"/>
+      <c r="L21" s="206"/>
       <c r="M21" s="26" t="s">
         <v>374</v>
       </c>
@@ -5090,7 +5101,7 @@
       <c r="AC21" s="106"/>
     </row>
     <row r="22" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="202"/>
+      <c r="A22" s="175"/>
       <c r="B22" s="91" t="s">
         <v>197</v>
       </c>
@@ -5104,7 +5115,7 @@
         <v>198</v>
       </c>
       <c r="F22" s="131"/>
-      <c r="L22" s="179"/>
+      <c r="L22" s="206"/>
       <c r="M22" s="26" t="s">
         <v>375</v>
       </c>
@@ -5134,23 +5145,23 @@
       <c r="AC22" s="106"/>
     </row>
     <row r="23" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="203" t="s">
+      <c r="A23" s="176" t="s">
         <v>200</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="211" t="s">
         <v>201</v>
       </c>
-      <c r="C23" s="33">
-        <v>1</v>
-      </c>
-      <c r="D23" s="33">
-        <v>1</v>
-      </c>
-      <c r="E23" s="29" t="s">
+      <c r="C23" s="212">
+        <v>1</v>
+      </c>
+      <c r="D23" s="212">
+        <v>0</v>
+      </c>
+      <c r="E23" s="213" t="s">
         <v>202</v>
       </c>
       <c r="F23" s="131"/>
-      <c r="L23" s="179"/>
+      <c r="L23" s="206"/>
       <c r="M23" s="109" t="s">
         <v>359</v>
       </c>
@@ -5180,7 +5191,7 @@
       <c r="AC23" s="106"/>
     </row>
     <row r="24" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="196"/>
+      <c r="A24" s="169"/>
       <c r="B24" s="26" t="s">
         <v>203</v>
       </c>
@@ -5194,7 +5205,7 @@
         <v>204</v>
       </c>
       <c r="F24" s="131"/>
-      <c r="L24" s="179"/>
+      <c r="L24" s="206"/>
       <c r="M24" s="26" t="s">
         <v>360</v>
       </c>
@@ -5224,7 +5235,7 @@
       <c r="AC24" s="106"/>
     </row>
     <row r="25" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="196"/>
+      <c r="A25" s="169"/>
       <c r="B25" s="26" t="s">
         <v>205</v>
       </c>
@@ -5238,7 +5249,7 @@
         <v>206</v>
       </c>
       <c r="F25" s="131"/>
-      <c r="L25" s="179"/>
+      <c r="L25" s="206"/>
       <c r="M25" s="71" t="s">
         <v>361</v>
       </c>
@@ -5262,7 +5273,7 @@
       <c r="AC25" s="106"/>
     </row>
     <row r="26" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="196"/>
+      <c r="A26" s="169"/>
       <c r="B26" s="26" t="s">
         <v>207</v>
       </c>
@@ -5276,7 +5287,7 @@
         <v>208</v>
       </c>
       <c r="F26" s="131"/>
-      <c r="L26" s="180"/>
+      <c r="L26" s="207"/>
       <c r="M26" s="74" t="s">
         <v>362</v>
       </c>
@@ -5302,7 +5313,7 @@
       <c r="AC26" s="106"/>
     </row>
     <row r="27" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="196"/>
+      <c r="A27" s="169"/>
       <c r="B27" s="26" t="s">
         <v>209</v>
       </c>
@@ -5316,7 +5327,7 @@
         <v>210</v>
       </c>
       <c r="F27" s="131"/>
-      <c r="L27" s="181" t="s">
+      <c r="L27" s="208" t="s">
         <v>213</v>
       </c>
       <c r="M27" s="84" t="s">
@@ -5348,7 +5359,7 @@
       <c r="AC27" s="106"/>
     </row>
     <row r="28" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="196"/>
+      <c r="A28" s="169"/>
       <c r="B28" s="78" t="s">
         <v>376</v>
       </c>
@@ -5362,7 +5373,7 @@
         <v>268</v>
       </c>
       <c r="F28" s="131"/>
-      <c r="L28" s="182"/>
+      <c r="L28" s="209"/>
       <c r="M28" s="26"/>
       <c r="N28" s="50"/>
       <c r="O28" s="50"/>
@@ -5384,7 +5395,7 @@
       <c r="AC28" s="106"/>
     </row>
     <row r="29" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="202"/>
+      <c r="A29" s="175"/>
       <c r="B29" s="136" t="s">
         <v>377</v>
       </c>
@@ -5398,7 +5409,7 @@
         <v>212</v>
       </c>
       <c r="F29" s="131"/>
-      <c r="L29" s="183"/>
+      <c r="L29" s="210"/>
       <c r="M29" s="113" t="s">
         <v>364</v>
       </c>
@@ -5422,7 +5433,7 @@
       <c r="AC29" s="106"/>
     </row>
     <row r="30" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="196" t="s">
+      <c r="A30" s="169" t="s">
         <v>213</v>
       </c>
       <c r="B30" s="26" t="s">
@@ -5457,7 +5468,7 @@
       <c r="AC30" s="106"/>
     </row>
     <row r="31" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="196"/>
+      <c r="A31" s="169"/>
       <c r="B31" s="26" t="s">
         <v>216</v>
       </c>
@@ -5494,7 +5505,7 @@
       <c r="AC31" s="106"/>
     </row>
     <row r="32" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="197"/>
+      <c r="A32" s="170"/>
       <c r="B32" s="42" t="s">
         <v>364</v>
       </c>
@@ -5558,27 +5569,27 @@
       <c r="AD33" s="93"/>
     </row>
     <row r="34" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="184" t="s">
+      <c r="B34" s="157" t="s">
         <v>295</v>
       </c>
-      <c r="C34" s="185"/>
-      <c r="D34" s="185"/>
-      <c r="E34" s="185"/>
-      <c r="F34" s="185"/>
-      <c r="G34" s="185"/>
-      <c r="H34" s="185"/>
-      <c r="I34" s="186"/>
+      <c r="C34" s="158"/>
+      <c r="D34" s="158"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="158"/>
+      <c r="G34" s="158"/>
+      <c r="H34" s="158"/>
+      <c r="I34" s="159"/>
       <c r="J34" s="142"/>
-      <c r="L34" s="175" t="s">
+      <c r="L34" s="202" t="s">
         <v>338</v>
       </c>
-      <c r="M34" s="176"/>
-      <c r="N34" s="176"/>
-      <c r="O34" s="176"/>
-      <c r="P34" s="176"/>
-      <c r="Q34" s="176"/>
-      <c r="R34" s="176"/>
-      <c r="S34" s="177"/>
+      <c r="M34" s="203"/>
+      <c r="N34" s="203"/>
+      <c r="O34" s="203"/>
+      <c r="P34" s="203"/>
+      <c r="Q34" s="203"/>
+      <c r="R34" s="203"/>
+      <c r="S34" s="204"/>
       <c r="U34" s="93"/>
       <c r="V34" s="93"/>
       <c r="W34" s="93"/>
@@ -7482,6 +7493,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="L4:P5"/>
+    <mergeCell ref="L7:L14"/>
+    <mergeCell ref="V4:Z5"/>
+    <mergeCell ref="V15:AC15"/>
+    <mergeCell ref="L34:S34"/>
+    <mergeCell ref="L15:L19"/>
+    <mergeCell ref="L20:L26"/>
+    <mergeCell ref="L27:L29"/>
     <mergeCell ref="B34:I34"/>
     <mergeCell ref="A1:F3"/>
     <mergeCell ref="A30:A32"/>
@@ -7494,14 +7513,6 @@
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="H1:J1"/>
-    <mergeCell ref="L4:P5"/>
-    <mergeCell ref="L7:L14"/>
-    <mergeCell ref="V4:Z5"/>
-    <mergeCell ref="V15:AC15"/>
-    <mergeCell ref="L34:S34"/>
-    <mergeCell ref="L15:L19"/>
-    <mergeCell ref="L20:L26"/>
-    <mergeCell ref="L27:L29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>